<commit_message>
630951 updated per reviewer comment
</commit_message>
<xml_diff>
--- a/Requirement/Build 6/TAS eBill RTM IB_2.0_608.xlsx
+++ b/Requirement/Build 6/TAS eBill RTM IB_2.0_608.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhaispbalchj\Documents\eBilling Docs\Build 5&amp;6\Docs\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VACOAPVCPM1001.dva.va.gov\FolderRedirection$\DVA\vacoclarkj5\Documents\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10344" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -321,9 +321,6 @@
     <t>DE487, DE528, DE748</t>
   </si>
   <si>
-    <t>IB*2.0*608_T31</t>
-  </si>
-  <si>
     <t>DE560, DE565, DE589, DE603, DE607, DE619, DE631, DE683, DE698</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>Updated to include retesting of Blds 3/4</t>
+  </si>
+  <si>
+    <t>IB*2.0*608_T33</t>
   </si>
 </sst>
 </file>
@@ -1627,14 +1627,14 @@
       <selection activeCell="A26" sqref="A26:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="21.109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="105" t="s">
         <v>0</v>
       </c>
@@ -1646,10 +1646,10 @@
       <c r="G5" s="105"/>
       <c r="H5" s="105"/>
     </row>
-    <row r="6" spans="1:8" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="106" t="s">
         <v>42</v>
       </c>
@@ -1661,51 +1661,51 @@
       <c r="G7" s="107"/>
       <c r="H7" s="107"/>
     </row>
-    <row r="8" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="108" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" s="108"/>
       <c r="C23" s="108"/>
@@ -1715,17 +1715,17 @@
       <c r="G23" s="108"/>
       <c r="H23" s="108"/>
     </row>
-    <row r="24" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="109" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="109"/>
       <c r="C26" s="109"/>
@@ -1735,22 +1735,22 @@
       <c r="G26" s="109"/>
       <c r="H26" s="109"/>
     </row>
-    <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
     </row>
-    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
     </row>
-    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
     </row>
   </sheetData>
@@ -1773,19 +1773,19 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" style="9" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="110" t="s">
         <v>1</v>
       </c>
@@ -1793,7 +1793,7 @@
       <c r="C2" s="110"/>
       <c r="D2" s="110"/>
     </row>
-    <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>76</v>
       </c>
@@ -1821,93 +1821,93 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="16" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="16" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="14">
         <v>2</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="20"/>
       <c r="C7" s="21"/>
       <c r="D7" s="22"/>
     </row>
-    <row r="8" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="23"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="22"/>
     </row>
-    <row r="9" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="22"/>
     </row>
-    <row r="10" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
       <c r="D10" s="22"/>
     </row>
-    <row r="11" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="22"/>
     </row>
-    <row r="12" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="21"/>
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
     </row>
-    <row r="13" spans="1:4" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
     </row>
   </sheetData>
@@ -1926,30 +1926,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DQ107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" style="29" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" style="34" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" style="34" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" style="34" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" style="33" customWidth="1"/>
-    <col min="11" max="11" width="29.109375" style="34" customWidth="1"/>
-    <col min="12" max="12" width="9.21875" style="33" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" style="34" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="33" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="34" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="34" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="34" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="34" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" style="33" customWidth="1"/>
+    <col min="11" max="11" width="29.140625" style="34" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" style="33" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="34" customWidth="1"/>
     <col min="14" max="14" width="26" style="33" customWidth="1"/>
-    <col min="15" max="16" width="8.88671875" style="33"/>
+    <col min="15" max="16" width="8.85546875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:121" s="47" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:121" s="47" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>7</v>
       </c>
@@ -2100,7 +2100,7 @@
       <c r="DP1" s="46"/>
       <c r="DQ1" s="46"/>
     </row>
-    <row r="2" spans="1:121" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:121" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>55</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="M2" s="49"/>
       <c r="N2" s="49"/>
     </row>
-    <row r="3" spans="1:121" s="103" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:121" s="103" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="99" t="s">
         <v>17</v>
       </c>
@@ -2150,19 +2150,19 @@
         <v>30</v>
       </c>
       <c r="K3" s="99" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L3" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="102" t="s">
-        <v>81</v>
+      <c r="M3" s="53" t="s">
+        <v>104</v>
       </c>
       <c r="N3" s="99" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:121" s="54" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:121" s="54" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
         <v>17</v>
       </c>
@@ -2200,15 +2200,15 @@
         <v>21</v>
       </c>
       <c r="M4" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" s="46" t="s">
         <v>81</v>
-      </c>
-      <c r="N4" s="46" t="s">
-        <v>82</v>
       </c>
       <c r="O4" s="46"/>
       <c r="P4" s="46"/>
     </row>
-    <row r="5" spans="1:121" s="54" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:121" s="54" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
         <v>17</v>
       </c>
@@ -2240,13 +2240,13 @@
         <v>30</v>
       </c>
       <c r="K5" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L5" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M5" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N5" s="46" t="s">
         <v>65</v>
@@ -2254,7 +2254,7 @@
       <c r="O5" s="46"/>
       <c r="P5" s="46"/>
     </row>
-    <row r="6" spans="1:121" s="54" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:121" s="54" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
         <v>17</v>
       </c>
@@ -2286,13 +2286,13 @@
         <v>30</v>
       </c>
       <c r="K6" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L6" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M6" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N6" s="46" t="s">
         <v>65</v>
@@ -2300,7 +2300,7 @@
       <c r="O6" s="46"/>
       <c r="P6" s="46"/>
     </row>
-    <row r="7" spans="1:121" s="54" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:121" s="54" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
         <v>17</v>
       </c>
@@ -2332,13 +2332,13 @@
         <v>30</v>
       </c>
       <c r="K7" s="98" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L7" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M7" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N7" s="46" t="s">
         <v>65</v>
@@ -2346,7 +2346,7 @@
       <c r="O7" s="46"/>
       <c r="P7" s="46"/>
     </row>
-    <row r="8" spans="1:121" s="54" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:121" s="54" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>17</v>
       </c>
@@ -2378,13 +2378,13 @@
         <v>30</v>
       </c>
       <c r="K8" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L8" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M8" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N8" s="46" t="s">
         <v>65</v>
@@ -2392,7 +2392,7 @@
       <c r="O8" s="46"/>
       <c r="P8" s="46"/>
     </row>
-    <row r="9" spans="1:121" s="54" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:121" s="54" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
         <v>17</v>
       </c>
@@ -2424,13 +2424,13 @@
         <v>30</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L9" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M9" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N9" s="46" t="s">
         <v>65</v>
@@ -2438,7 +2438,7 @@
       <c r="O9" s="46"/>
       <c r="P9" s="46"/>
     </row>
-    <row r="10" spans="1:121" s="54" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:121" s="54" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
         <v>17</v>
       </c>
@@ -2470,13 +2470,13 @@
         <v>30</v>
       </c>
       <c r="K10" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L10" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M10" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N10" s="46" t="s">
         <v>65</v>
@@ -2484,7 +2484,7 @@
       <c r="O10" s="46"/>
       <c r="P10" s="46"/>
     </row>
-    <row r="11" spans="1:121" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:121" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
@@ -2502,7 +2502,7 @@
       <c r="O11" s="46"/>
       <c r="P11" s="46"/>
     </row>
-    <row r="12" spans="1:121" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:121" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
         <v>58</v>
       </c>
@@ -2520,7 +2520,7 @@
       <c r="M12" s="49"/>
       <c r="N12" s="49"/>
     </row>
-    <row r="13" spans="1:121" s="54" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:121" s="54" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
         <v>17</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>21</v>
       </c>
       <c r="M13" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N13" s="46" t="s">
         <v>60</v>
@@ -2566,7 +2566,7 @@
       <c r="O13" s="46"/>
       <c r="P13" s="46"/>
     </row>
-    <row r="14" spans="1:121" s="54" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:121" s="54" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
         <v>17</v>
       </c>
@@ -2598,13 +2598,13 @@
         <v>30</v>
       </c>
       <c r="K14" s="40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L14" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N14" s="46" t="s">
         <v>65</v>
@@ -2612,7 +2612,7 @@
       <c r="O14" s="46"/>
       <c r="P14" s="46"/>
     </row>
-    <row r="15" spans="1:121" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:121" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="55"/>
       <c r="B15" s="46"/>
       <c r="C15" s="46"/>
@@ -2630,7 +2630,7 @@
       <c r="O15" s="46"/>
       <c r="P15" s="46"/>
     </row>
-    <row r="16" spans="1:121" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:121" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
         <v>36</v>
       </c>
@@ -2648,7 +2648,7 @@
       <c r="M16" s="49"/>
       <c r="N16" s="49"/>
     </row>
-    <row r="17" spans="1:121" s="54" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:121" s="54" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
         <v>17</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>21</v>
       </c>
       <c r="M17" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N17" s="46" t="s">
         <v>50</v>
@@ -2694,7 +2694,7 @@
       <c r="O17" s="46"/>
       <c r="P17" s="46"/>
     </row>
-    <row r="18" spans="1:121" s="54" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:121" s="54" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
         <v>17</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>21</v>
       </c>
       <c r="M18" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N18" s="46" t="s">
         <v>80</v>
@@ -2740,7 +2740,7 @@
       <c r="O18" s="46"/>
       <c r="P18" s="46"/>
     </row>
-    <row r="19" spans="1:121" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:121" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
       <c r="B19" s="46"/>
       <c r="C19" s="56"/>
@@ -2758,7 +2758,7 @@
       <c r="O19" s="46"/>
       <c r="P19" s="46"/>
     </row>
-    <row r="20" spans="1:121" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:121" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>27</v>
       </c>
@@ -2883,7 +2883,7 @@
       <c r="DP20" s="60"/>
       <c r="DQ20" s="60"/>
     </row>
-    <row r="21" spans="1:121" s="54" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:121" s="54" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
         <v>17</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>21</v>
       </c>
       <c r="M21" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N21" s="64" t="s">
         <v>17</v>
@@ -2929,7 +2929,7 @@
       <c r="O21" s="41"/>
       <c r="P21" s="46"/>
     </row>
-    <row r="22" spans="1:121" s="54" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:121" s="54" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
         <v>17</v>
       </c>
@@ -2961,13 +2961,13 @@
         <v>30</v>
       </c>
       <c r="K22" s="63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L22" s="63" t="s">
         <v>21</v>
       </c>
       <c r="M22" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N22" s="64" t="s">
         <v>65</v>
@@ -2975,7 +2975,7 @@
       <c r="O22" s="41"/>
       <c r="P22" s="46"/>
     </row>
-    <row r="23" spans="1:121" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:121" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="63"/>
       <c r="B23" s="63"/>
       <c r="C23" s="62"/>
@@ -2993,7 +2993,7 @@
       <c r="O23" s="41"/>
       <c r="P23" s="46"/>
     </row>
-    <row r="24" spans="1:121" s="111" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:121" s="111" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="111" t="s">
         <v>32</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="DP24" s="112"/>
       <c r="DQ24" s="112"/>
     </row>
-    <row r="25" spans="1:121" s="73" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:121" s="73" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="66" t="s">
         <v>17</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>21</v>
       </c>
       <c r="M25" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N25" s="66" t="s">
         <v>74</v>
@@ -3164,7 +3164,7 @@
       <c r="O25" s="72"/>
       <c r="P25" s="72"/>
     </row>
-    <row r="26" spans="1:121" s="73" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:121" s="73" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="66" t="s">
         <v>17</v>
       </c>
@@ -3196,11 +3196,11 @@
         <v>30</v>
       </c>
       <c r="K26" s="66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L26" s="57"/>
       <c r="M26" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N26" s="66" t="s">
         <v>65</v>
@@ -3208,7 +3208,7 @@
       <c r="O26" s="72"/>
       <c r="P26" s="72"/>
     </row>
-    <row r="27" spans="1:121" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:121" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
       <c r="B27" s="35"/>
       <c r="C27" s="56"/>
@@ -3226,7 +3226,7 @@
       <c r="O27" s="74"/>
       <c r="P27" s="74"/>
     </row>
-    <row r="28" spans="1:121" s="111" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:121" s="111" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="111" t="s">
         <v>66</v>
       </c>
@@ -3351,7 +3351,7 @@
       <c r="DP28" s="112"/>
       <c r="DQ28" s="112"/>
     </row>
-    <row r="29" spans="1:121" s="104" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:121" s="104" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>17</v>
       </c>
@@ -3383,19 +3383,19 @@
         <v>30</v>
       </c>
       <c r="K29" s="100" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L29" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M29" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N29" s="100" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:121" s="75" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
         <v>17</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>21</v>
       </c>
       <c r="M30" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N30" s="35" t="s">
         <v>72</v>
@@ -3441,7 +3441,7 @@
       <c r="O30" s="74"/>
       <c r="P30" s="74"/>
     </row>
-    <row r="31" spans="1:121" s="75" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
         <v>17</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>21</v>
       </c>
       <c r="M31" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N31" s="35" t="s">
         <v>75</v>
@@ -3487,7 +3487,7 @@
       <c r="O31" s="74"/>
       <c r="P31" s="74"/>
     </row>
-    <row r="32" spans="1:121" s="75" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
         <v>17</v>
       </c>
@@ -3519,13 +3519,13 @@
         <v>30</v>
       </c>
       <c r="K32" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L32" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M32" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N32" s="35" t="s">
         <v>65</v>
@@ -3533,7 +3533,7 @@
       <c r="O32" s="74"/>
       <c r="P32" s="74"/>
     </row>
-    <row r="33" spans="1:121" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:121" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35"/>
       <c r="B33" s="35"/>
       <c r="C33" s="56"/>
@@ -3551,7 +3551,7 @@
       <c r="O33" s="74"/>
       <c r="P33" s="74"/>
     </row>
-    <row r="34" spans="1:121" s="111" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:121" s="111" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="111" t="s">
         <v>51</v>
       </c>
@@ -3676,7 +3676,7 @@
       <c r="DP34" s="112"/>
       <c r="DQ34" s="112"/>
     </row>
-    <row r="35" spans="1:121" s="75" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="66" t="s">
         <v>17</v>
       </c>
@@ -3708,13 +3708,13 @@
         <v>30</v>
       </c>
       <c r="K35" s="40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L35" s="57" t="s">
         <v>21</v>
       </c>
       <c r="M35" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N35" s="53" t="s">
         <v>64</v>
@@ -3722,7 +3722,7 @@
       <c r="O35" s="74"/>
       <c r="P35" s="74"/>
     </row>
-    <row r="36" spans="1:121" s="75" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="66" t="s">
         <v>17</v>
       </c>
@@ -3754,13 +3754,13 @@
         <v>30</v>
       </c>
       <c r="K36" s="56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L36" s="57" t="s">
         <v>21</v>
       </c>
       <c r="M36" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N36" s="35" t="s">
         <v>65</v>
@@ -3768,7 +3768,7 @@
       <c r="O36" s="74"/>
       <c r="P36" s="74"/>
     </row>
-    <row r="37" spans="1:121" s="75" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="66" t="s">
         <v>17</v>
       </c>
@@ -3800,13 +3800,13 @@
         <v>30</v>
       </c>
       <c r="K37" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L37" s="57" t="s">
         <v>21</v>
       </c>
       <c r="M37" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N37" s="35" t="s">
         <v>63</v>
@@ -3814,7 +3814,7 @@
       <c r="O37" s="74"/>
       <c r="P37" s="74"/>
     </row>
-    <row r="38" spans="1:121" s="75" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="66" t="s">
         <v>17</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>21</v>
       </c>
       <c r="M38" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N38" s="35" t="s">
         <v>54</v>
@@ -3860,7 +3860,7 @@
       <c r="O38" s="74"/>
       <c r="P38" s="74"/>
     </row>
-    <row r="39" spans="1:121" s="75" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="66" t="s">
         <v>17</v>
       </c>
@@ -3892,13 +3892,13 @@
         <v>30</v>
       </c>
       <c r="K39" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L39" s="57" t="s">
         <v>21</v>
       </c>
       <c r="M39" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N39" s="35" t="s">
         <v>65</v>
@@ -3906,7 +3906,7 @@
       <c r="O39" s="74"/>
       <c r="P39" s="74"/>
     </row>
-    <row r="40" spans="1:121" s="75" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="66" t="s">
         <v>17</v>
       </c>
@@ -3938,13 +3938,13 @@
         <v>30</v>
       </c>
       <c r="K40" s="35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L40" s="57" t="s">
         <v>21</v>
       </c>
       <c r="M40" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N40" s="35" t="s">
         <v>65</v>
@@ -3952,7 +3952,7 @@
       <c r="O40" s="74"/>
       <c r="P40" s="74"/>
     </row>
-    <row r="41" spans="1:121" s="75" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="66" t="s">
         <v>17</v>
       </c>
@@ -3984,13 +3984,13 @@
         <v>30</v>
       </c>
       <c r="K41" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L41" s="57" t="s">
         <v>21</v>
       </c>
       <c r="M41" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N41" s="35" t="s">
         <v>65</v>
@@ -3998,7 +3998,7 @@
       <c r="O41" s="74"/>
       <c r="P41" s="74"/>
     </row>
-    <row r="42" spans="1:121" s="75" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:121" s="75" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="66" t="s">
         <v>17</v>
       </c>
@@ -4030,13 +4030,13 @@
         <v>30</v>
       </c>
       <c r="K42" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L42" s="53" t="s">
         <v>21</v>
       </c>
       <c r="M42" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N42" s="35" t="s">
         <v>65</v>
@@ -4044,7 +4044,7 @@
       <c r="O42" s="74"/>
       <c r="P42" s="74"/>
     </row>
-    <row r="43" spans="1:121" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:121" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="66"/>
       <c r="B43" s="35"/>
       <c r="C43" s="56"/>
@@ -4062,7 +4062,7 @@
       <c r="O43" s="74"/>
       <c r="P43" s="74"/>
     </row>
-    <row r="44" spans="1:121" s="111" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:121" s="111" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="111" t="s">
         <v>46</v>
       </c>
@@ -4187,7 +4187,7 @@
       <c r="DP44" s="112"/>
       <c r="DQ44" s="112"/>
     </row>
-    <row r="45" spans="1:121" s="74" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:121" s="74" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
         <v>17</v>
       </c>
@@ -4225,13 +4225,13 @@
         <v>21</v>
       </c>
       <c r="M45" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N45" s="35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:121" s="75" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:121" s="75" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>17</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>21</v>
       </c>
       <c r="M46" s="53" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="N46" s="35" t="s">
         <v>17</v>
@@ -4277,7 +4277,7 @@
       <c r="O46" s="74"/>
       <c r="P46" s="74"/>
     </row>
-    <row r="47" spans="1:121" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:121" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35"/>
       <c r="B47" s="35"/>
       <c r="C47" s="35"/>
@@ -4295,7 +4295,7 @@
       <c r="O47" s="77"/>
       <c r="P47" s="77"/>
     </row>
-    <row r="48" spans="1:121" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:121" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="35"/>
       <c r="B48" s="35"/>
       <c r="C48" s="35"/>
@@ -4313,7 +4313,7 @@
       <c r="O48" s="77"/>
       <c r="P48" s="77"/>
     </row>
-    <row r="49" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="35"/>
       <c r="B49" s="35"/>
       <c r="C49" s="35"/>
@@ -4331,7 +4331,7 @@
       <c r="O49" s="77"/>
       <c r="P49" s="77"/>
     </row>
-    <row r="50" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="35"/>
       <c r="B50" s="35"/>
       <c r="C50" s="35"/>
@@ -4349,7 +4349,7 @@
       <c r="O50" s="77"/>
       <c r="P50" s="77"/>
     </row>
-    <row r="51" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="35"/>
       <c r="B51" s="35"/>
       <c r="C51" s="35"/>
@@ -4367,7 +4367,7 @@
       <c r="O51" s="77"/>
       <c r="P51" s="77"/>
     </row>
-    <row r="52" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="35"/>
       <c r="B52" s="35"/>
       <c r="C52" s="35"/>
@@ -4385,7 +4385,7 @@
       <c r="O52" s="77"/>
       <c r="P52" s="77"/>
     </row>
-    <row r="53" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="35"/>
       <c r="B53" s="35"/>
       <c r="C53" s="35"/>
@@ -4403,7 +4403,7 @@
       <c r="O53" s="77"/>
       <c r="P53" s="77"/>
     </row>
-    <row r="54" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="35"/>
       <c r="B54" s="35"/>
       <c r="C54" s="35"/>
@@ -4421,7 +4421,7 @@
       <c r="O54" s="77"/>
       <c r="P54" s="77"/>
     </row>
-    <row r="55" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="35"/>
       <c r="B55" s="35"/>
       <c r="C55" s="35"/>
@@ -4439,7 +4439,7 @@
       <c r="O55" s="77"/>
       <c r="P55" s="77"/>
     </row>
-    <row r="56" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35"/>
       <c r="B56" s="35"/>
       <c r="C56" s="35"/>
@@ -4457,7 +4457,7 @@
       <c r="O56" s="77"/>
       <c r="P56" s="77"/>
     </row>
-    <row r="57" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="35"/>
       <c r="B57" s="35"/>
       <c r="C57" s="35"/>
@@ -4475,7 +4475,7 @@
       <c r="O57" s="77"/>
       <c r="P57" s="77"/>
     </row>
-    <row r="58" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="35"/>
       <c r="B58" s="35"/>
       <c r="C58" s="35"/>
@@ -4493,7 +4493,7 @@
       <c r="O58" s="77"/>
       <c r="P58" s="77"/>
     </row>
-    <row r="59" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="41"/>
       <c r="B59" s="41"/>
       <c r="C59" s="41"/>
@@ -4511,7 +4511,7 @@
       <c r="O59" s="79"/>
       <c r="P59" s="79"/>
     </row>
-    <row r="60" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="41"/>
       <c r="B60" s="41"/>
       <c r="C60" s="41"/>
@@ -4529,7 +4529,7 @@
       <c r="O60" s="79"/>
       <c r="P60" s="79"/>
     </row>
-    <row r="61" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="41"/>
       <c r="B61" s="41"/>
       <c r="C61" s="41"/>
@@ -4547,7 +4547,7 @@
       <c r="O61" s="79"/>
       <c r="P61" s="79"/>
     </row>
-    <row r="62" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="41"/>
       <c r="B62" s="41"/>
       <c r="C62" s="41"/>
@@ -4565,7 +4565,7 @@
       <c r="O62" s="79"/>
       <c r="P62" s="79"/>
     </row>
-    <row r="63" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="41"/>
       <c r="B63" s="41"/>
       <c r="C63" s="41"/>
@@ -4583,7 +4583,7 @@
       <c r="O63" s="79"/>
       <c r="P63" s="79"/>
     </row>
-    <row r="64" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="41"/>
       <c r="B64" s="41"/>
       <c r="C64" s="41"/>
@@ -4601,7 +4601,7 @@
       <c r="O64" s="79"/>
       <c r="P64" s="79"/>
     </row>
-    <row r="65" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="41"/>
       <c r="B65" s="41"/>
       <c r="C65" s="41"/>
@@ -4619,7 +4619,7 @@
       <c r="O65" s="79"/>
       <c r="P65" s="79"/>
     </row>
-    <row r="66" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="41"/>
       <c r="B66" s="41"/>
       <c r="C66" s="41"/>
@@ -4637,7 +4637,7 @@
       <c r="O66" s="79"/>
       <c r="P66" s="79"/>
     </row>
-    <row r="67" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="41"/>
       <c r="B67" s="41"/>
       <c r="C67" s="41"/>
@@ -4655,7 +4655,7 @@
       <c r="O67" s="79"/>
       <c r="P67" s="79"/>
     </row>
-    <row r="68" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="41"/>
       <c r="B68" s="41"/>
       <c r="C68" s="41"/>
@@ -4673,7 +4673,7 @@
       <c r="O68" s="79"/>
       <c r="P68" s="79"/>
     </row>
-    <row r="69" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="41"/>
       <c r="B69" s="41"/>
       <c r="C69" s="41"/>
@@ -4691,7 +4691,7 @@
       <c r="O69" s="79"/>
       <c r="P69" s="79"/>
     </row>
-    <row r="70" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="41"/>
       <c r="B70" s="41"/>
       <c r="C70" s="41"/>
@@ -4709,7 +4709,7 @@
       <c r="O70" s="79"/>
       <c r="P70" s="79"/>
     </row>
-    <row r="71" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="41"/>
       <c r="B71" s="41"/>
       <c r="C71" s="41"/>
@@ -4727,7 +4727,7 @@
       <c r="O71" s="79"/>
       <c r="P71" s="79"/>
     </row>
-    <row r="72" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="79"/>
       <c r="B72" s="79"/>
       <c r="C72" s="79"/>
@@ -4745,7 +4745,7 @@
       <c r="O72" s="79"/>
       <c r="P72" s="79"/>
     </row>
-    <row r="73" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="79"/>
       <c r="B73" s="79"/>
       <c r="C73" s="79"/>
@@ -4763,7 +4763,7 @@
       <c r="O73" s="79"/>
       <c r="P73" s="79"/>
     </row>
-    <row r="74" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="79"/>
       <c r="B74" s="79"/>
       <c r="C74" s="79"/>
@@ -4781,7 +4781,7 @@
       <c r="O74" s="79"/>
       <c r="P74" s="79"/>
     </row>
-    <row r="75" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="79"/>
       <c r="B75" s="79"/>
       <c r="C75" s="79"/>
@@ -4799,7 +4799,7 @@
       <c r="O75" s="79"/>
       <c r="P75" s="79"/>
     </row>
-    <row r="76" spans="1:16" s="85" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="84"/>
       <c r="B76" s="84"/>
       <c r="C76" s="79"/>
@@ -4817,7 +4817,7 @@
       <c r="O76" s="84"/>
       <c r="P76" s="84"/>
     </row>
-    <row r="77" spans="1:16" s="85" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" s="85" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="84"/>
       <c r="B77" s="84"/>
       <c r="C77" s="79"/>
@@ -4835,7 +4835,7 @@
       <c r="O77" s="84"/>
       <c r="P77" s="84"/>
     </row>
-    <row r="78" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="84"/>
       <c r="B78" s="84"/>
       <c r="C78" s="79"/>
@@ -4853,7 +4853,7 @@
       <c r="O78" s="84"/>
       <c r="P78" s="84"/>
     </row>
-    <row r="79" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" s="86" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="84"/>
       <c r="B79" s="84"/>
       <c r="C79" s="79"/>
@@ -4871,7 +4871,7 @@
       <c r="O79" s="84"/>
       <c r="P79" s="84"/>
     </row>
-    <row r="80" spans="1:16" s="89" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" s="89" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="87"/>
       <c r="B80" s="87"/>
       <c r="C80" s="88"/>
@@ -4889,7 +4889,7 @@
       <c r="O80" s="87"/>
       <c r="P80" s="87"/>
     </row>
-    <row r="81" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="90"/>
       <c r="B81" s="90"/>
       <c r="C81" s="91"/>
@@ -4907,7 +4907,7 @@
       <c r="O81" s="90"/>
       <c r="P81" s="90"/>
     </row>
-    <row r="82" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="90"/>
       <c r="B82" s="90"/>
       <c r="C82" s="91"/>
@@ -4925,7 +4925,7 @@
       <c r="O82" s="90"/>
       <c r="P82" s="90"/>
     </row>
-    <row r="83" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="90"/>
       <c r="B83" s="90"/>
       <c r="C83" s="91"/>
@@ -4943,7 +4943,7 @@
       <c r="O83" s="90"/>
       <c r="P83" s="90"/>
     </row>
-    <row r="84" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="90"/>
       <c r="B84" s="90"/>
       <c r="C84" s="91"/>
@@ -4961,7 +4961,7 @@
       <c r="O84" s="90"/>
       <c r="P84" s="90"/>
     </row>
-    <row r="85" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="90"/>
       <c r="B85" s="90"/>
       <c r="C85" s="91"/>
@@ -4979,7 +4979,7 @@
       <c r="O85" s="90"/>
       <c r="P85" s="90"/>
     </row>
-    <row r="86" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="90"/>
       <c r="B86" s="90"/>
       <c r="C86" s="91"/>
@@ -4997,7 +4997,7 @@
       <c r="O86" s="90"/>
       <c r="P86" s="90"/>
     </row>
-    <row r="87" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="90"/>
       <c r="B87" s="90"/>
       <c r="C87" s="91"/>
@@ -5015,7 +5015,7 @@
       <c r="O87" s="90"/>
       <c r="P87" s="90"/>
     </row>
-    <row r="88" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="90"/>
       <c r="B88" s="90"/>
       <c r="C88" s="91"/>
@@ -5033,7 +5033,7 @@
       <c r="O88" s="90"/>
       <c r="P88" s="90"/>
     </row>
-    <row r="89" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" s="93" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="90"/>
       <c r="B89" s="90"/>
       <c r="C89" s="91"/>
@@ -5051,13 +5051,13 @@
       <c r="O89" s="90"/>
       <c r="P89" s="90"/>
     </row>
-    <row r="90" spans="1:16" s="90" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" s="90" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C90" s="91"/>
       <c r="F90" s="92"/>
       <c r="K90" s="91"/>
       <c r="M90" s="91"/>
     </row>
-    <row r="91" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="30"/>
       <c r="B91" s="30"/>
       <c r="C91" s="31"/>
@@ -5075,7 +5075,7 @@
       <c r="O91" s="30"/>
       <c r="P91" s="30"/>
     </row>
-    <row r="92" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="30"/>
       <c r="B92" s="30"/>
       <c r="C92" s="31"/>
@@ -5093,7 +5093,7 @@
       <c r="O92" s="30"/>
       <c r="P92" s="30"/>
     </row>
-    <row r="93" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="30"/>
       <c r="B93" s="30"/>
       <c r="C93" s="31"/>
@@ -5111,7 +5111,7 @@
       <c r="O93" s="30"/>
       <c r="P93" s="30"/>
     </row>
-    <row r="94" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="30"/>
       <c r="B94" s="30"/>
       <c r="C94" s="31"/>
@@ -5129,7 +5129,7 @@
       <c r="O94" s="30"/>
       <c r="P94" s="30"/>
     </row>
-    <row r="95" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="30"/>
       <c r="B95" s="30"/>
       <c r="C95" s="31"/>
@@ -5147,7 +5147,7 @@
       <c r="O95" s="30"/>
       <c r="P95" s="30"/>
     </row>
-    <row r="96" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="30"/>
       <c r="B96" s="30"/>
       <c r="C96" s="31"/>
@@ -5165,7 +5165,7 @@
       <c r="O96" s="30"/>
       <c r="P96" s="30"/>
     </row>
-    <row r="97" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="30"/>
       <c r="B97" s="30"/>
       <c r="C97" s="31"/>
@@ -5183,7 +5183,7 @@
       <c r="O97" s="30"/>
       <c r="P97" s="30"/>
     </row>
-    <row r="98" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="30"/>
       <c r="B98" s="30"/>
       <c r="C98" s="31"/>
@@ -5201,7 +5201,7 @@
       <c r="O98" s="30"/>
       <c r="P98" s="30"/>
     </row>
-    <row r="99" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="30"/>
       <c r="B99" s="30"/>
       <c r="C99" s="31"/>
@@ -5219,7 +5219,7 @@
       <c r="O99" s="30"/>
       <c r="P99" s="30"/>
     </row>
-    <row r="100" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="39"/>
       <c r="B100" s="30"/>
       <c r="C100" s="31"/>
@@ -5237,7 +5237,7 @@
       <c r="O100" s="30"/>
       <c r="P100" s="30"/>
     </row>
-    <row r="101" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="30"/>
       <c r="B101" s="30"/>
       <c r="C101" s="31"/>
@@ -5255,7 +5255,7 @@
       <c r="O101" s="30"/>
       <c r="P101" s="30"/>
     </row>
-    <row r="102" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="30"/>
       <c r="B102" s="30"/>
       <c r="C102" s="31"/>
@@ -5273,7 +5273,7 @@
       <c r="O102" s="30"/>
       <c r="P102" s="30"/>
     </row>
-    <row r="103" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="30"/>
       <c r="B103" s="30"/>
       <c r="C103" s="31"/>
@@ -5291,7 +5291,7 @@
       <c r="O103" s="30"/>
       <c r="P103" s="30"/>
     </row>
-    <row r="104" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="30"/>
       <c r="B104" s="30"/>
       <c r="C104" s="31"/>
@@ -5309,7 +5309,7 @@
       <c r="O104" s="30"/>
       <c r="P104" s="30"/>
     </row>
-    <row r="105" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="30"/>
       <c r="B105" s="30"/>
       <c r="C105" s="31"/>
@@ -5327,7 +5327,7 @@
       <c r="O105" s="30"/>
       <c r="P105" s="30"/>
     </row>
-    <row r="106" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="30"/>
       <c r="B106" s="30"/>
       <c r="C106" s="31"/>
@@ -5345,7 +5345,7 @@
       <c r="O106" s="30"/>
       <c r="P106" s="30"/>
     </row>
-    <row r="107" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="30"/>
       <c r="B107" s="30"/>
       <c r="C107" s="31"/>

</xml_diff>